<commit_message>
- improve excel illustration
</commit_message>
<xml_diff>
--- a/excel/Übung1Aufgabe2.xlsx
+++ b/excel/Übung1Aufgabe2.xlsx
@@ -46,7 +46,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="0.0000000000000000000000000"/>
+    <numFmt numFmtId="164" formatCode="0.0000000000000000000000000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -79,7 +79,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -679,11 +679,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1505578576"/>
-        <c:axId val="-1428956848"/>
+        <c:axId val="2129254832"/>
+        <c:axId val="2129256464"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1505578576"/>
+        <c:axId val="2129254832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -691,7 +691,7 @@
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
+        <c:tickLblPos val="low"/>
         <c:spPr>
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -724,7 +724,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1428956848"/>
+        <c:crossAx val="2129256464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -732,7 +732,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1428956848"/>
+        <c:axId val="2129256464"/>
         <c:scaling>
           <c:logBase val="2"/>
           <c:orientation val="minMax"/>
@@ -783,7 +783,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1505578576"/>
+        <c:crossAx val="2129254832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>

</xml_diff>